<commit_message>
Improved performance, added extra features for GUI
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -2389,7 +2389,7 @@
       </c>
       <c r="AD2" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">التميمي ومشاركوه للمحاماة واإلستشارات     </t>
+          <t xml:space="preserve">التميمي ومشاركوه للمحاماة والاستشارات     </t>
         </is>
       </c>
       <c r="AF2" s="9" t="inlineStr">
@@ -12829,7 +12829,7 @@
       </c>
       <c r="AD155" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">للمحاماة واإلستشارات   التميمي ومشاركوه    </t>
+          <t xml:space="preserve">للمحاماة والاستشارات   التميمي ومشاركوه    </t>
         </is>
       </c>
       <c r="AF155" s="9" t="inlineStr">
@@ -13863,7 +13863,7 @@
       </c>
       <c r="AD170" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">التميمي ومشاركوه للمحاماة واإلستشارات     </t>
+          <t xml:space="preserve">التميمي ومشاركوه للمحاماة والاستشارات     </t>
         </is>
       </c>
       <c r="AF170" s="9" t="inlineStr">
@@ -13931,7 +13931,7 @@
       </c>
       <c r="AD171" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">التميمي ومشاركوه للمحاماة واإلستشارات     </t>
+          <t xml:space="preserve">التميمي ومشاركوه للمحاماة والاستشارات     </t>
         </is>
       </c>
       <c r="AF171" s="9" t="inlineStr">
@@ -13999,7 +13999,7 @@
       </c>
       <c r="AD172" s="9" t="inlineStr">
         <is>
-          <t xml:space="preserve">التميمي ومشاركوه للمحاماة واإلستشارات     </t>
+          <t xml:space="preserve">التميمي ومشاركوه للمحاماة والاستشارات     </t>
         </is>
       </c>
       <c r="AF172" s="9" t="inlineStr">

</xml_diff>